<commit_message>
Fixed some code for creating sequential table.
</commit_message>
<xml_diff>
--- a/sequential_table.xlsx
+++ b/sequential_table.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F1"/>
+  <dimension ref="A1:F11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -465,6 +465,266 @@
         </is>
       </c>
     </row>
+    <row r="2">
+      <c r="A2" t="n">
+        <v>1</v>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>first-year</t>
+        </is>
+      </c>
+      <c r="C2" t="n">
+        <v>0</v>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>True: In Java, every variable has a type that is known at compile time.</t>
+        </is>
+      </c>
+      <c r="E2" t="inlineStr">
+        <is>
+          <t>Correct</t>
+        </is>
+      </c>
+      <c r="F2" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="n">
+        <v>2</v>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>first-year</t>
+        </is>
+      </c>
+      <c r="C3" t="n">
+        <v>0</v>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>False: In Java, the result of applying one of the arithmetic operators to two double operands may produce a run-time exception if the operands cause an overflow or underflow.</t>
+        </is>
+      </c>
+      <c r="E3" t="inlineStr">
+        <is>
+          <t>Incorrect</t>
+        </is>
+      </c>
+      <c r="F3" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="n">
+        <v>3</v>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>first-year</t>
+        </is>
+      </c>
+      <c r="C4" t="n">
+        <v>0</v>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>False: In Java, if you attempt to use a local variable of type int in an expression before that variable has been assigned a value, Java will throw a compile-time error.</t>
+        </is>
+      </c>
+      <c r="E4" t="inlineStr">
+        <is>
+          <t>Correct</t>
+        </is>
+      </c>
+      <c r="F4" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="n">
+        <v>4</v>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>first-year</t>
+        </is>
+      </c>
+      <c r="C5" t="n">
+        <v>0</v>
+      </c>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>True: In Java, if a variable is declared and initialized in the body of a for loop, that variable cannot be accessed outside that loop.</t>
+        </is>
+      </c>
+      <c r="E5" t="inlineStr">
+        <is>
+          <t>Correct</t>
+        </is>
+      </c>
+      <c r="F5" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="n">
+        <v>5</v>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>first-year</t>
+        </is>
+      </c>
+      <c r="C6" t="n">
+        <v>0</v>
+      </c>
+      <c r="D6" t="inlineStr">
+        <is>
+          <t>False: In Java, if you name a variable with all uppercase letters and initialize it to some value, attempting to subsequently change its value would not lead to a compile-time error, but it is not a good naming convention.</t>
+        </is>
+      </c>
+      <c r="E6" t="inlineStr">
+        <is>
+          <t>Correct</t>
+        </is>
+      </c>
+      <c r="F6" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="n">
+        <v>6</v>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>first-year</t>
+        </is>
+      </c>
+      <c r="C7" t="n">
+        <v>0</v>
+      </c>
+      <c r="D7" t="inlineStr">
+        <is>
+          <t>False: In Java, after you create and initialize an int[] array, you can change its length by using the method Array.resize().</t>
+        </is>
+      </c>
+      <c r="E7" t="inlineStr">
+        <is>
+          <t>Incorrect</t>
+        </is>
+      </c>
+      <c r="F7" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="n">
+        <v>7</v>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>first-year</t>
+        </is>
+      </c>
+      <c r="C8" t="n">
+        <v>0</v>
+      </c>
+      <c r="D8" t="inlineStr">
+        <is>
+          <t>False: In Java, a[0.0] is not a valid expression that gives the first element of an array of type char[], but a[0] does give the first element.</t>
+        </is>
+      </c>
+      <c r="E8" t="inlineStr">
+        <is>
+          <t>Correct</t>
+        </is>
+      </c>
+      <c r="F8" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="n">
+        <v>8</v>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>first-year</t>
+        </is>
+      </c>
+      <c r="C9" t="n">
+        <v>0</v>
+      </c>
+      <c r="D9" t="inlineStr">
+        <is>
+          <t>False: In Java, it is not possible to declare, create, and initialize a String[] array without using the keyword new.</t>
+        </is>
+      </c>
+      <c r="E9" t="inlineStr">
+        <is>
+          <t>Incorrect</t>
+        </is>
+      </c>
+      <c r="F9" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="n">
+        <v>9</v>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>first-year</t>
+        </is>
+      </c>
+      <c r="C10" t="n">
+        <v>0</v>
+      </c>
+      <c r="D10" t="inlineStr">
+        <is>
+          <t>False: In Java, if a[] and b[] are two different arrays of the same type and length, then the expression (a == b) evaluates to false, even if the corresponding array elements are equal.</t>
+        </is>
+      </c>
+      <c r="E10" t="inlineStr">
+        <is>
+          <t>Correct</t>
+        </is>
+      </c>
+      <c r="F10" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="n">
+        <v>10</v>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>first-year</t>
+        </is>
+      </c>
+      <c r="C11" t="n">
+        <v>0</v>
+      </c>
+      <c r="D11" t="inlineStr">
+        <is>
+          <t>True: In Java, the elements of an array of type int[] are stored contiguously in the computer’s memory (i.e., in consecutive memory locations).</t>
+        </is>
+      </c>
+      <c r="E11" t="inlineStr">
+        <is>
+          <t>Correct</t>
+        </is>
+      </c>
+      <c r="F11" t="n">
+        <v>1</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>